<commit_message>
ran the v1 script
</commit_message>
<xml_diff>
--- a/data/final/FINAL_CAR_with_gpdg_pcp.xlsx
+++ b/data/final/FINAL_CAR_with_gpdg_pcp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b407939\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b407939\Documents\GitHub\MA\data\final\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -5132,12 +5132,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AW302"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AN168" sqref="AN168"/>
+      <selection pane="bottomLeft" activeCell="AN1" sqref="AN1:AN1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5316,7 +5315,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -5465,7 +5464,7 @@
         <v>64.333068764608996</v>
       </c>
     </row>
-    <row r="3" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -5614,7 +5613,7 @@
         <v>64.333068764608996</v>
       </c>
     </row>
-    <row r="4" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>76</v>
       </c>
@@ -5763,7 +5762,7 @@
         <v>104.74176255873</v>
       </c>
     </row>
-    <row r="5" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -6061,7 +6060,7 @@
         <v>64.333068764608996</v>
       </c>
     </row>
-    <row r="7" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>103</v>
       </c>
@@ -6210,7 +6209,7 @@
         <v>39.801623574722001</v>
       </c>
     </row>
-    <row r="8" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>111</v>
       </c>
@@ -6359,7 +6358,7 @@
         <v>64.333068764608996</v>
       </c>
     </row>
-    <row r="9" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>117</v>
       </c>
@@ -6508,7 +6507,7 @@
         <v>44.048516434673999</v>
       </c>
     </row>
-    <row r="10" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -6657,7 +6656,7 @@
         <v>39.801623574722001</v>
       </c>
     </row>
-    <row r="11" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>129</v>
       </c>
@@ -6806,7 +6805,7 @@
         <v>66.460091756926005</v>
       </c>
     </row>
-    <row r="12" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>135</v>
       </c>
@@ -6955,7 +6954,7 @@
         <v>41.000351027953997</v>
       </c>
     </row>
-    <row r="13" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>139</v>
       </c>
@@ -7253,7 +7252,7 @@
         <v>68.038767657376994</v>
       </c>
     </row>
-    <row r="15" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>155</v>
       </c>
@@ -7402,7 +7401,7 @@
         <v>66.460091756926005</v>
       </c>
     </row>
-    <row r="16" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>160</v>
       </c>
@@ -7551,7 +7550,7 @@
         <v>41.000351027953997</v>
       </c>
     </row>
-    <row r="17" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>166</v>
       </c>
@@ -7700,7 +7699,7 @@
         <v>54.890007155532999</v>
       </c>
     </row>
-    <row r="18" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>170</v>
       </c>
@@ -7849,7 +7848,7 @@
         <v>66.460091756926005</v>
       </c>
     </row>
-    <row r="19" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>177</v>
       </c>
@@ -7998,7 +7997,7 @@
         <v>95.141870163883993</v>
       </c>
     </row>
-    <row r="20" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>184</v>
       </c>
@@ -8147,7 +8146,7 @@
         <v>41.000351027953997</v>
       </c>
     </row>
-    <row r="21" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>189</v>
       </c>
@@ -8296,7 +8295,7 @@
         <v>41.000351027953997</v>
       </c>
     </row>
-    <row r="22" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>195</v>
       </c>
@@ -8445,7 +8444,7 @@
         <v>65.754024845641993</v>
       </c>
     </row>
-    <row r="23" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>201</v>
       </c>
@@ -8594,7 +8593,7 @@
         <v>42.058357189149</v>
       </c>
     </row>
-    <row r="24" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>205</v>
       </c>
@@ -8743,7 +8742,7 @@
         <v>42.058357189149</v>
       </c>
     </row>
-    <row r="25" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>211</v>
       </c>
@@ -8892,7 +8891,7 @@
         <v>48.46713125566</v>
       </c>
     </row>
-    <row r="26" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>217</v>
       </c>
@@ -9041,7 +9040,7 @@
         <v>106.25306955972</v>
       </c>
     </row>
-    <row r="27" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>223</v>
       </c>
@@ -9190,7 +9189,7 @@
         <v>65.324748897681999</v>
       </c>
     </row>
-    <row r="28" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>229</v>
       </c>
@@ -9488,7 +9487,7 @@
         <v>48.46713125566</v>
       </c>
     </row>
-    <row r="30" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>237</v>
       </c>
@@ -9637,7 +9636,7 @@
         <v>31.493577776959999</v>
       </c>
     </row>
-    <row r="31" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>241</v>
       </c>
@@ -9786,7 +9785,7 @@
         <v>43.173897815474</v>
       </c>
     </row>
-    <row r="32" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>247</v>
       </c>
@@ -9935,7 +9934,7 @@
         <v>43.173897815474</v>
       </c>
     </row>
-    <row r="33" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>255</v>
       </c>
@@ -10084,7 +10083,7 @@
         <v>63.081440630629999</v>
       </c>
     </row>
-    <row r="34" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>261</v>
       </c>
@@ -10233,7 +10232,7 @@
         <v>65.361396134667999</v>
       </c>
     </row>
-    <row r="35" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>267</v>
       </c>
@@ -10382,7 +10381,7 @@
         <v>49.515078125595998</v>
       </c>
     </row>
-    <row r="36" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>274</v>
       </c>
@@ -10531,7 +10530,7 @@
         <v>43.173897815474</v>
       </c>
     </row>
-    <row r="37" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>278</v>
       </c>
@@ -10680,7 +10679,7 @@
         <v>42.741118381438</v>
       </c>
     </row>
-    <row r="38" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>286</v>
       </c>
@@ -10978,7 +10977,7 @@
         <v>39.072554361199003</v>
       </c>
     </row>
-    <row r="40" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>295</v>
       </c>
@@ -11127,7 +11126,7 @@
         <v>43.173897815474</v>
       </c>
     </row>
-    <row r="41" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>303</v>
       </c>
@@ -11425,7 +11424,7 @@
         <v>63.081440630629999</v>
       </c>
     </row>
-    <row r="43" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>314</v>
       </c>
@@ -11574,7 +11573,7 @@
         <v>44.751849868378997</v>
       </c>
     </row>
-    <row r="44" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>320</v>
       </c>
@@ -11872,7 +11871,7 @@
         <v>93.160043440931005</v>
       </c>
     </row>
-    <row r="46" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>328</v>
       </c>
@@ -12021,7 +12020,7 @@
         <v>64.586203700843001</v>
       </c>
     </row>
-    <row r="47" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>332</v>
       </c>
@@ -12170,7 +12169,7 @@
         <v>64.586203700843001</v>
       </c>
     </row>
-    <row r="48" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>339</v>
       </c>
@@ -12319,7 +12318,7 @@
         <v>105.78767746274001</v>
       </c>
     </row>
-    <row r="49" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>343</v>
       </c>
@@ -12468,7 +12467,7 @@
         <v>105.78767746274001</v>
       </c>
     </row>
-    <row r="50" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>347</v>
       </c>
@@ -12617,7 +12616,7 @@
         <v>50.827371987951999</v>
       </c>
     </row>
-    <row r="51" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>351</v>
       </c>
@@ -12766,7 +12765,7 @@
         <v>69.735692990293003</v>
       </c>
     </row>
-    <row r="52" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>355</v>
       </c>
@@ -13064,7 +13063,7 @@
         <v>105.78767746274001</v>
       </c>
     </row>
-    <row r="54" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>367</v>
       </c>
@@ -13213,7 +13212,7 @@
         <v>43.087987059162998</v>
       </c>
     </row>
-    <row r="55" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>371</v>
       </c>
@@ -13362,7 +13361,7 @@
         <v>71.715680576542994</v>
       </c>
     </row>
-    <row r="56" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>375</v>
       </c>
@@ -13511,7 +13510,7 @@
         <v>116.12127583182</v>
       </c>
     </row>
-    <row r="57" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>381</v>
       </c>
@@ -13660,7 +13659,7 @@
         <v>40.947598349171997</v>
       </c>
     </row>
-    <row r="58" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>389</v>
       </c>
@@ -13809,7 +13808,7 @@
         <v>53.079279210430997</v>
       </c>
     </row>
-    <row r="59" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>396</v>
       </c>
@@ -13958,7 +13957,7 @@
         <v>64.915011731647994</v>
       </c>
     </row>
-    <row r="60" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>400</v>
       </c>
@@ -14256,7 +14255,7 @@
         <v>71.715680576542994</v>
       </c>
     </row>
-    <row r="62" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>410</v>
       </c>
@@ -14554,7 +14553,7 @@
         <v>40.947598349171997</v>
       </c>
     </row>
-    <row r="64" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>420</v>
       </c>
@@ -14703,7 +14702,7 @@
         <v>64.915011731647994</v>
       </c>
     </row>
-    <row r="65" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>426</v>
       </c>
@@ -14852,7 +14851,7 @@
         <v>71.715680576542994</v>
       </c>
     </row>
-    <row r="66" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>432</v>
       </c>
@@ -15150,7 +15149,7 @@
         <v>80.375526555201006</v>
       </c>
     </row>
-    <row r="68" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>440</v>
       </c>
@@ -15299,7 +15298,7 @@
         <v>75.860229659824995</v>
       </c>
     </row>
-    <row r="69" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>444</v>
       </c>
@@ -15597,7 +15596,7 @@
         <v>80.375526555201006</v>
       </c>
     </row>
-    <row r="71" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>452</v>
       </c>
@@ -15746,7 +15745,7 @@
         <v>86.134992773790003</v>
       </c>
     </row>
-    <row r="72" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>459</v>
       </c>
@@ -15895,7 +15894,7 @@
         <v>86.313311004070002</v>
       </c>
     </row>
-    <row r="73" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>463</v>
       </c>
@@ -16044,7 +16043,7 @@
         <v>80.375526555201006</v>
       </c>
     </row>
-    <row r="74" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>467</v>
       </c>
@@ -16193,7 +16192,7 @@
         <v>86.134992773790003</v>
       </c>
     </row>
-    <row r="75" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>471</v>
       </c>
@@ -16342,7 +16341,7 @@
         <v>80.375526555201006</v>
       </c>
     </row>
-    <row r="76" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>475</v>
       </c>
@@ -16491,7 +16490,7 @@
         <v>61.166928094413002</v>
       </c>
     </row>
-    <row r="77" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>479</v>
       </c>
@@ -16640,7 +16639,7 @@
         <v>81.425065710728006</v>
       </c>
     </row>
-    <row r="78" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>483</v>
       </c>
@@ -16938,7 +16937,7 @@
         <v>81.425065710728006</v>
       </c>
     </row>
-    <row r="80" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>493</v>
       </c>
@@ -17236,7 +17235,7 @@
         <v>81.425065710728006</v>
       </c>
     </row>
-    <row r="82" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>501</v>
       </c>
@@ -17385,7 +17384,7 @@
         <v>81.425065710728006</v>
       </c>
     </row>
-    <row r="83" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>505</v>
       </c>
@@ -17534,7 +17533,7 @@
         <v>84.482600665804995</v>
       </c>
     </row>
-    <row r="84" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>509</v>
       </c>
@@ -17683,7 +17682,7 @@
         <v>89.560379607786004</v>
       </c>
     </row>
-    <row r="85" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>516</v>
       </c>
@@ -17832,7 +17831,7 @@
         <v>91.717557032637004</v>
       </c>
     </row>
-    <row r="86" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>522</v>
       </c>
@@ -17981,7 +17980,7 @@
         <v>125.87049589393</v>
       </c>
     </row>
-    <row r="87" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>529</v>
       </c>
@@ -18130,7 +18129,7 @@
         <v>84.482600665804995</v>
       </c>
     </row>
-    <row r="88" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>533</v>
       </c>
@@ -18279,7 +18278,7 @@
         <v>79.157292938815004</v>
       </c>
     </row>
-    <row r="89" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>537</v>
       </c>
@@ -18428,7 +18427,7 @@
         <v>42.569499885417997</v>
       </c>
     </row>
-    <row r="90" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>541</v>
       </c>
@@ -18577,7 +18576,7 @@
         <v>37.686333135723999</v>
       </c>
     </row>
-    <row r="91" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>547</v>
       </c>
@@ -18726,7 +18725,7 @@
         <v>84.482600665804995</v>
       </c>
     </row>
-    <row r="92" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>553</v>
       </c>
@@ -18875,7 +18874,7 @@
         <v>118.72991735162999</v>
       </c>
     </row>
-    <row r="93" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>557</v>
       </c>
@@ -19173,7 +19172,7 @@
         <v>84.482600665804995</v>
       </c>
     </row>
-    <row r="95" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>567</v>
       </c>
@@ -19322,7 +19321,7 @@
         <v>76.794662537318004</v>
       </c>
     </row>
-    <row r="96" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>571</v>
       </c>
@@ -19769,7 +19768,7 @@
         <v>85.316058901030999</v>
       </c>
     </row>
-    <row r="99" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>583</v>
       </c>
@@ -19918,7 +19917,7 @@
         <v>131.81630273306001</v>
       </c>
     </row>
-    <row r="100" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>590</v>
       </c>
@@ -20216,7 +20215,7 @@
         <v>100.00031287415</v>
       </c>
     </row>
-    <row r="102" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>598</v>
       </c>
@@ -20365,7 +20364,7 @@
         <v>76.794662537318004</v>
       </c>
     </row>
-    <row r="103" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>604</v>
       </c>
@@ -20812,7 +20811,7 @@
         <v>94.686825462051004</v>
       </c>
     </row>
-    <row r="106" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>618</v>
       </c>
@@ -20961,7 +20960,7 @@
         <v>42.066967582149999</v>
       </c>
     </row>
-    <row r="107" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>622</v>
       </c>
@@ -21110,7 +21109,7 @@
         <v>96.317504471418999</v>
       </c>
     </row>
-    <row r="108" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>626</v>
       </c>
@@ -21259,7 +21258,7 @@
         <v>87.094325197019003</v>
       </c>
     </row>
-    <row r="109" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>631</v>
       </c>
@@ -21408,7 +21407,7 @@
         <v>104.41761636037999</v>
       </c>
     </row>
-    <row r="110" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>637</v>
       </c>
@@ -21557,7 +21556,7 @@
         <v>67.165909991792006</v>
       </c>
     </row>
-    <row r="111" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>641</v>
       </c>
@@ -21855,7 +21854,7 @@
         <v>73.823031854131997</v>
       </c>
     </row>
-    <row r="113" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>649</v>
       </c>
@@ -22302,7 +22301,7 @@
         <v>104.41761636037999</v>
       </c>
     </row>
-    <row r="116" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>663</v>
       </c>
@@ -22749,7 +22748,7 @@
         <v>87.094325197019003</v>
       </c>
     </row>
-    <row r="119" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>677</v>
       </c>
@@ -22898,7 +22897,7 @@
         <v>44.290452475480997</v>
       </c>
     </row>
-    <row r="120" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>681</v>
       </c>
@@ -23047,7 +23046,7 @@
         <v>87.094325197019003</v>
       </c>
     </row>
-    <row r="121" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>685</v>
       </c>
@@ -23196,7 +23195,7 @@
         <v>67.165909991792006</v>
       </c>
     </row>
-    <row r="122" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>689</v>
       </c>
@@ -23494,7 +23493,7 @@
         <v>44.035592881896001</v>
       </c>
     </row>
-    <row r="124" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>699</v>
       </c>
@@ -23643,7 +23642,7 @@
         <v>39.894178226248997</v>
       </c>
     </row>
-    <row r="125" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>703</v>
       </c>
@@ -23792,7 +23791,7 @@
         <v>102.44212445452</v>
       </c>
     </row>
-    <row r="126" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>707</v>
       </c>
@@ -23941,7 +23940,7 @@
         <v>63.799334930454002</v>
       </c>
     </row>
-    <row r="127" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>713</v>
       </c>
@@ -24388,7 +24387,7 @@
         <v>102.44212445452</v>
       </c>
     </row>
-    <row r="130" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>729</v>
       </c>
@@ -24537,7 +24536,7 @@
         <v>44.035592881896001</v>
       </c>
     </row>
-    <row r="131" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>735</v>
       </c>
@@ -24686,7 +24685,7 @@
         <v>42.157849611921002</v>
       </c>
     </row>
-    <row r="132" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>739</v>
       </c>
@@ -24984,7 +24983,7 @@
         <v>44.035592881896001</v>
       </c>
     </row>
-    <row r="134" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>751</v>
       </c>
@@ -25133,7 +25132,7 @@
         <v>87.866686912423006</v>
       </c>
     </row>
-    <row r="135" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>755</v>
       </c>
@@ -25282,7 +25281,7 @@
         <v>87.866686912423006</v>
       </c>
     </row>
-    <row r="136" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>759</v>
       </c>
@@ -25580,7 +25579,7 @@
         <v>98.024778336433997</v>
       </c>
     </row>
-    <row r="138" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>768</v>
       </c>
@@ -25729,7 +25728,7 @@
         <v>42.373485372264</v>
       </c>
     </row>
-    <row r="139" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>772</v>
       </c>
@@ -25878,7 +25877,7 @@
         <v>42.373485372264</v>
       </c>
     </row>
-    <row r="140" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>776</v>
       </c>
@@ -26027,7 +26026,7 @@
         <v>67.630651010134002</v>
       </c>
     </row>
-    <row r="141" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>780</v>
       </c>
@@ -26176,7 +26175,7 @@
         <v>37.304314351366997</v>
       </c>
     </row>
-    <row r="142" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>786</v>
       </c>
@@ -26325,7 +26324,7 @@
         <v>68.591112896444002</v>
       </c>
     </row>
-    <row r="143" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>794</v>
       </c>
@@ -26474,7 +26473,7 @@
         <v>42.373485372264</v>
       </c>
     </row>
-    <row r="144" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>798</v>
       </c>
@@ -26623,7 +26622,7 @@
         <v>82.840428625757994</v>
       </c>
     </row>
-    <row r="145" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>803</v>
       </c>
@@ -26772,7 +26771,7 @@
         <v>67.630651010134002</v>
       </c>
     </row>
-    <row r="146" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>807</v>
       </c>
@@ -26921,7 +26920,7 @@
         <v>105.00714974947</v>
       </c>
     </row>
-    <row r="147" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>811</v>
       </c>
@@ -27219,7 +27218,7 @@
         <v>67.630651010134002</v>
       </c>
     </row>
-    <row r="149" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>819</v>
       </c>
@@ -27368,7 +27367,7 @@
         <v>101.96650275565</v>
       </c>
     </row>
-    <row r="150" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>823</v>
       </c>
@@ -27666,7 +27665,7 @@
         <v>40.936561690761998</v>
       </c>
     </row>
-    <row r="152" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>833</v>
       </c>
@@ -27815,7 +27814,7 @@
         <v>98.024778336433997</v>
       </c>
     </row>
-    <row r="153" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>837</v>
       </c>
@@ -27964,7 +27963,7 @@
         <v>131.50574455009999</v>
       </c>
     </row>
-    <row r="154" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>843</v>
       </c>
@@ -28113,7 +28112,7 @@
         <v>102.02179530390001</v>
       </c>
     </row>
-    <row r="155" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>848</v>
       </c>
@@ -28411,7 +28410,7 @@
         <v>63.952376234949</v>
       </c>
     </row>
-    <row r="157" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>858</v>
       </c>
@@ -28560,7 +28559,7 @@
         <v>66.512105153766996</v>
       </c>
     </row>
-    <row r="158" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>864</v>
       </c>
@@ -28709,7 +28708,7 @@
         <v>63.952376234949</v>
       </c>
     </row>
-    <row r="159" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>868</v>
       </c>
@@ -28858,7 +28857,7 @@
         <v>183.20543380767</v>
       </c>
     </row>
-    <row r="160" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>877</v>
       </c>
@@ -29007,7 +29006,7 @@
         <v>101.14423857972</v>
       </c>
     </row>
-    <row r="161" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>881</v>
       </c>
@@ -29156,7 +29155,7 @@
         <v>41.753380143385002</v>
       </c>
     </row>
-    <row r="162" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>887</v>
       </c>
@@ -29305,7 +29304,7 @@
         <v>101.14423857972</v>
       </c>
     </row>
-    <row r="163" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>891</v>
       </c>
@@ -29454,7 +29453,7 @@
         <v>86.72315054824</v>
       </c>
     </row>
-    <row r="164" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>895</v>
       </c>
@@ -29603,7 +29602,7 @@
         <v>86.72315054824</v>
       </c>
     </row>
-    <row r="165" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>899</v>
       </c>
@@ -29752,7 +29751,7 @@
         <v>65.2783212983</v>
       </c>
     </row>
-    <row r="166" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>905</v>
       </c>
@@ -29901,7 +29900,7 @@
         <v>51.557591839171003</v>
       </c>
     </row>
-    <row r="167" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>909</v>
       </c>
@@ -30199,7 +30198,7 @@
         <v>60.728535497052</v>
       </c>
     </row>
-    <row r="169" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>917</v>
       </c>
@@ -30348,7 +30347,7 @@
         <v>39.784001691699999</v>
       </c>
     </row>
-    <row r="170" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>921</v>
       </c>
@@ -30497,7 +30496,7 @@
         <v>65.2783212983</v>
       </c>
     </row>
-    <row r="171" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>927</v>
       </c>
@@ -30646,7 +30645,7 @@
         <v>86.345469784936995</v>
       </c>
     </row>
-    <row r="172" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>931</v>
       </c>
@@ -31242,7 +31241,7 @@
         <v>39.784001691699999</v>
       </c>
     </row>
-    <row r="176" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>949</v>
       </c>
@@ -31391,7 +31390,7 @@
         <v>98.159104237877003</v>
       </c>
     </row>
-    <row r="177" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>955</v>
       </c>
@@ -31540,7 +31539,7 @@
         <v>86.345469784936995</v>
       </c>
     </row>
-    <row r="178" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>959</v>
       </c>
@@ -31689,7 +31688,7 @@
         <v>65.241487437770999</v>
       </c>
     </row>
-    <row r="179" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>963</v>
       </c>
@@ -31838,7 +31837,7 @@
         <v>58.556132032771004</v>
       </c>
     </row>
-    <row r="180" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>969</v>
       </c>
@@ -31987,7 +31986,7 @@
         <v>97.885860680536993</v>
       </c>
     </row>
-    <row r="181" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>973</v>
       </c>
@@ -32136,7 +32135,7 @@
         <v>35.695844772653999</v>
       </c>
     </row>
-    <row r="182" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>978</v>
       </c>
@@ -32285,7 +32284,7 @@
         <v>85.657505345980994</v>
       </c>
     </row>
-    <row r="183" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>984</v>
       </c>
@@ -32583,7 +32582,7 @@
         <v>97.885860680536993</v>
       </c>
     </row>
-    <row r="185" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>995</v>
       </c>
@@ -32732,7 +32731,7 @@
         <v>65.241487437770999</v>
       </c>
     </row>
-    <row r="186" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>999</v>
       </c>
@@ -32881,7 +32880,7 @@
         <v>65.241487437770999</v>
       </c>
     </row>
-    <row r="187" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>1002</v>
       </c>
@@ -33030,7 +33029,7 @@
         <v>97.885860680536993</v>
       </c>
     </row>
-    <row r="188" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>1006</v>
       </c>
@@ -33328,7 +33327,7 @@
         <v>58.556132032771004</v>
       </c>
     </row>
-    <row r="190" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>1016</v>
       </c>
@@ -33477,7 +33476,7 @@
         <v>133.82273913911999</v>
       </c>
     </row>
-    <row r="191" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>1022</v>
       </c>
@@ -33626,7 +33625,7 @@
         <v>35.695844772653999</v>
       </c>
     </row>
-    <row r="192" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>1027</v>
       </c>
@@ -33775,7 +33774,7 @@
         <v>85.657505345980994</v>
       </c>
     </row>
-    <row r="193" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>1033</v>
       </c>
@@ -33924,7 +33923,7 @@
         <v>35.695844772653999</v>
       </c>
     </row>
-    <row r="194" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>1039</v>
       </c>
@@ -34073,7 +34072,7 @@
         <v>35.695844772653999</v>
       </c>
     </row>
-    <row r="195" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>1043</v>
       </c>
@@ -34222,7 +34221,7 @@
         <v>85.657505345980994</v>
       </c>
     </row>
-    <row r="196" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>1047</v>
       </c>
@@ -34371,7 +34370,7 @@
         <v>47.582634643219002</v>
       </c>
     </row>
-    <row r="197" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>1053</v>
       </c>
@@ -34520,7 +34519,7 @@
         <v>85.657505345980994</v>
       </c>
     </row>
-    <row r="198" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>1059</v>
       </c>
@@ -34669,7 +34668,7 @@
         <v>58.556132032771004</v>
       </c>
     </row>
-    <row r="199" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>1063</v>
       </c>
@@ -34818,7 +34817,7 @@
         <v>67.858169885378999</v>
       </c>
     </row>
-    <row r="200" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>1068</v>
       </c>
@@ -34967,7 +34966,7 @@
         <v>105.80010911054001</v>
       </c>
     </row>
-    <row r="201" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>1072</v>
       </c>
@@ -35116,7 +35115,7 @@
         <v>75.260353152594007</v>
       </c>
     </row>
-    <row r="202" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>1078</v>
       </c>
@@ -35265,7 +35264,7 @@
         <v>114.85301782010001</v>
       </c>
     </row>
-    <row r="203" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>1082</v>
       </c>
@@ -35414,7 +35413,7 @@
         <v>114.85301782010001</v>
       </c>
     </row>
-    <row r="204" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>1088</v>
       </c>
@@ -35563,7 +35562,7 @@
         <v>43.198776482207002</v>
       </c>
     </row>
-    <row r="205" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>1092</v>
       </c>
@@ -35712,7 +35711,7 @@
         <v>40.311887445036</v>
       </c>
     </row>
-    <row r="206" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>1098</v>
       </c>
@@ -35861,7 +35860,7 @@
         <v>67.858169885378999</v>
       </c>
     </row>
-    <row r="207" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>1102</v>
       </c>
@@ -36159,7 +36158,7 @@
         <v>154.28804453106</v>
       </c>
     </row>
-    <row r="209" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>1112</v>
       </c>
@@ -36308,7 +36307,7 @@
         <v>57.007189840034002</v>
       </c>
     </row>
-    <row r="210" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>1116</v>
       </c>
@@ -36457,7 +36456,7 @@
         <v>43.198776482207002</v>
       </c>
     </row>
-    <row r="211" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>1122</v>
       </c>
@@ -36755,7 +36754,7 @@
         <v>82.947875047980006</v>
       </c>
     </row>
-    <row r="213" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>1134</v>
       </c>
@@ -36904,7 +36903,7 @@
         <v>67.858169885378999</v>
       </c>
     </row>
-    <row r="214" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>1138</v>
       </c>
@@ -37053,7 +37052,7 @@
         <v>105.80010911054001</v>
       </c>
     </row>
-    <row r="215" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>1142</v>
       </c>
@@ -37202,7 +37201,7 @@
         <v>67.858169885378999</v>
       </c>
     </row>
-    <row r="216" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>1146</v>
       </c>
@@ -37500,7 +37499,7 @@
         <v>105.80010911054001</v>
       </c>
     </row>
-    <row r="218" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>1156</v>
       </c>
@@ -37649,7 +37648,7 @@
         <v>67.858169885378999</v>
       </c>
     </row>
-    <row r="219" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>1160</v>
       </c>
@@ -37798,7 +37797,7 @@
         <v>105.80010911054001</v>
       </c>
     </row>
-    <row r="220" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>1164</v>
       </c>
@@ -37947,7 +37946,7 @@
         <v>154.28804453106</v>
       </c>
     </row>
-    <row r="221" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>1170</v>
       </c>
@@ -38096,7 +38095,7 @@
         <v>40.311887445036</v>
       </c>
     </row>
-    <row r="222" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>1174</v>
       </c>
@@ -38245,7 +38244,7 @@
         <v>82.947875047980006</v>
       </c>
     </row>
-    <row r="223" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>1178</v>
       </c>
@@ -38394,7 +38393,7 @@
         <v>105.80010911054001</v>
       </c>
     </row>
-    <row r="224" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>1184</v>
       </c>
@@ -38543,7 +38542,7 @@
         <v>114.85301782010001</v>
       </c>
     </row>
-    <row r="225" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>1190</v>
       </c>
@@ -38692,7 +38691,7 @@
         <v>67.858169885378999</v>
       </c>
     </row>
-    <row r="226" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>1194</v>
       </c>
@@ -38841,7 +38840,7 @@
         <v>82.947875047980006</v>
       </c>
     </row>
-    <row r="227" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>1197</v>
       </c>
@@ -38990,7 +38989,7 @@
         <v>67.858169885378999</v>
       </c>
     </row>
-    <row r="228" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>1203</v>
       </c>
@@ -39139,7 +39138,7 @@
         <v>105.80010911054001</v>
       </c>
     </row>
-    <row r="229" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>1207</v>
       </c>
@@ -39288,7 +39287,7 @@
         <v>105.80010911054001</v>
       </c>
     </row>
-    <row r="230" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>1210</v>
       </c>
@@ -39437,7 +39436,7 @@
         <v>41.641192156210003</v>
       </c>
     </row>
-    <row r="231" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>1214</v>
       </c>
@@ -39586,7 +39585,7 @@
         <v>113.08790347100999</v>
       </c>
     </row>
-    <row r="232" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>1218</v>
       </c>
@@ -39735,7 +39734,7 @@
         <v>115.59391415764</v>
       </c>
     </row>
-    <row r="233" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>1223</v>
       </c>
@@ -39884,7 +39883,7 @@
         <v>67.878829091027995</v>
       </c>
     </row>
-    <row r="234" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>1226</v>
       </c>
@@ -40033,7 +40032,7 @@
         <v>115.59391415764</v>
       </c>
     </row>
-    <row r="235" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>1230</v>
       </c>
@@ -40182,7 +40181,7 @@
         <v>105.19601117124</v>
       </c>
     </row>
-    <row r="236" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>1236</v>
       </c>
@@ -40331,7 +40330,7 @@
         <v>36.833662831508001</v>
       </c>
     </row>
-    <row r="237" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>1242</v>
       </c>
@@ -40480,7 +40479,7 @@
         <v>105.19601117124</v>
       </c>
     </row>
-    <row r="238" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>1246</v>
       </c>
@@ -40629,7 +40628,7 @@
         <v>105.19601117124</v>
       </c>
     </row>
-    <row r="239" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>1252</v>
       </c>
@@ -40778,7 +40777,7 @@
         <v>36.833662831508001</v>
       </c>
     </row>
-    <row r="240" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>1256</v>
       </c>
@@ -40927,7 +40926,7 @@
         <v>107.93525199680001</v>
       </c>
     </row>
-    <row r="241" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>1262</v>
       </c>
@@ -41076,7 +41075,7 @@
         <v>145.73468991087</v>
       </c>
     </row>
-    <row r="242" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>1266</v>
       </c>
@@ -41225,7 +41224,7 @@
         <v>50.435645785429998</v>
       </c>
     </row>
-    <row r="243" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>1272</v>
       </c>
@@ -41374,7 +41373,7 @@
         <v>115.59391415764</v>
       </c>
     </row>
-    <row r="244" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>1278</v>
       </c>
@@ -41523,7 +41522,7 @@
         <v>115.59391415764</v>
       </c>
     </row>
-    <row r="245" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>1284</v>
       </c>
@@ -41672,7 +41671,7 @@
         <v>50.435645785429998</v>
       </c>
     </row>
-    <row r="246" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>1290</v>
       </c>
@@ -41821,7 +41820,7 @@
         <v>105.19601117124</v>
       </c>
     </row>
-    <row r="247" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>1294</v>
       </c>
@@ -41970,7 +41969,7 @@
         <v>40.980865664706002</v>
       </c>
     </row>
-    <row r="248" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>1300</v>
       </c>
@@ -42268,7 +42267,7 @@
         <v>145.73468991087</v>
       </c>
     </row>
-    <row r="250" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>1310</v>
       </c>
@@ -42417,7 +42416,7 @@
         <v>105.19601117124</v>
       </c>
     </row>
-    <row r="251" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>1314</v>
       </c>
@@ -42566,7 +42565,7 @@
         <v>36.833662831508001</v>
       </c>
     </row>
-    <row r="252" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>1320</v>
       </c>
@@ -42715,7 +42714,7 @@
         <v>67.878829091027995</v>
       </c>
     </row>
-    <row r="253" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>1324</v>
       </c>
@@ -42864,7 +42863,7 @@
         <v>40.980865664706002</v>
       </c>
     </row>
-    <row r="254" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>1330</v>
       </c>
@@ -43013,7 +43012,7 @@
         <v>67.878829091027995</v>
       </c>
     </row>
-    <row r="255" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>1336</v>
       </c>
@@ -43162,7 +43161,7 @@
         <v>105.19601117124</v>
       </c>
     </row>
-    <row r="256" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>1342</v>
       </c>
@@ -43311,7 +43310,7 @@
         <v>105.19601117124</v>
       </c>
     </row>
-    <row r="257" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>1348</v>
       </c>
@@ -43460,7 +43459,7 @@
         <v>105.19601117124</v>
       </c>
     </row>
-    <row r="258" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>1355</v>
       </c>
@@ -43609,7 +43608,7 @@
         <v>145.73468991087</v>
       </c>
     </row>
-    <row r="259" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>1359</v>
       </c>
@@ -43758,7 +43757,7 @@
         <v>40.980865664706002</v>
       </c>
     </row>
-    <row r="260" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>1363</v>
       </c>
@@ -43907,7 +43906,7 @@
         <v>50.435645785429998</v>
       </c>
     </row>
-    <row r="261" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>1367</v>
       </c>
@@ -44056,7 +44055,7 @@
         <v>50.435645785429998</v>
       </c>
     </row>
-    <row r="262" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>1373</v>
       </c>
@@ -44205,7 +44204,7 @@
         <v>40.980865664706002</v>
       </c>
     </row>
-    <row r="263" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>1379</v>
       </c>
@@ -44354,7 +44353,7 @@
         <v>115.59391415764</v>
       </c>
     </row>
-    <row r="264" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>1383</v>
       </c>
@@ -44503,7 +44502,7 @@
         <v>100.43232570399</v>
       </c>
     </row>
-    <row r="265" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>1387</v>
       </c>
@@ -44652,7 +44651,7 @@
         <v>33.752971546974003</v>
       </c>
     </row>
-    <row r="266" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>1391</v>
       </c>
@@ -44801,7 +44800,7 @@
         <v>100.43232570399</v>
       </c>
     </row>
-    <row r="267" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>1395</v>
       </c>
@@ -44950,7 +44949,7 @@
         <v>36.270510219437</v>
       </c>
     </row>
-    <row r="268" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>1401</v>
       </c>
@@ -45099,7 +45098,7 @@
         <v>100.43232570399</v>
       </c>
     </row>
-    <row r="269" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>1405</v>
       </c>
@@ -45248,7 +45247,7 @@
         <v>111.95130179017001</v>
       </c>
     </row>
-    <row r="270" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>1411</v>
       </c>
@@ -45397,7 +45396,7 @@
         <v>33.752971546974003</v>
       </c>
     </row>
-    <row r="271" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>1416</v>
       </c>
@@ -45546,7 +45545,7 @@
         <v>33.752971546974003</v>
       </c>
     </row>
-    <row r="272" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>1422</v>
       </c>
@@ -45695,7 +45694,7 @@
         <v>111.95130179017001</v>
       </c>
     </row>
-    <row r="273" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>1426</v>
       </c>
@@ -45844,7 +45843,7 @@
         <v>43.143073237403001</v>
       </c>
     </row>
-    <row r="274" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>1430</v>
       </c>
@@ -45993,7 +45992,7 @@
         <v>37.194739974862998</v>
       </c>
     </row>
-    <row r="275" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>1434</v>
       </c>
@@ -46142,7 +46141,7 @@
         <v>37.194739974862998</v>
       </c>
     </row>
-    <row r="276" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>1438</v>
       </c>
@@ -46291,7 +46290,7 @@
         <v>104.28155910894</v>
       </c>
     </row>
-    <row r="277" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>1442</v>
       </c>
@@ -46440,7 +46439,7 @@
         <v>48.353625405003001</v>
       </c>
     </row>
-    <row r="278" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>1448</v>
       </c>
@@ -46589,7 +46588,7 @@
         <v>33.752971546974003</v>
       </c>
     </row>
-    <row r="279" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>1454</v>
       </c>
@@ -46738,7 +46737,7 @@
         <v>33.752971546974003</v>
       </c>
     </row>
-    <row r="280" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>1460</v>
       </c>
@@ -46887,7 +46886,7 @@
         <v>64.789357208796005</v>
       </c>
     </row>
-    <row r="281" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>1466</v>
       </c>
@@ -47036,7 +47035,7 @@
         <v>29.698146562089999</v>
       </c>
     </row>
-    <row r="282" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
         <v>1470</v>
       </c>
@@ -47185,7 +47184,7 @@
         <v>100.43232570399</v>
       </c>
     </row>
-    <row r="283" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
         <v>1474</v>
       </c>
@@ -47334,7 +47333,7 @@
         <v>100.43232570399</v>
       </c>
     </row>
-    <row r="284" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
         <v>1480</v>
       </c>
@@ -47781,7 +47780,7 @@
         <v>111.95130179017001</v>
       </c>
     </row>
-    <row r="287" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
         <v>1492</v>
       </c>
@@ -47930,7 +47929,7 @@
         <v>48.353625405003001</v>
       </c>
     </row>
-    <row r="288" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
         <v>1496</v>
       </c>
@@ -48228,7 +48227,7 @@
         <v>36.37122985845</v>
       </c>
     </row>
-    <row r="290" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
         <v>1506</v>
       </c>
@@ -48377,7 +48376,7 @@
         <v>101.14707428398999</v>
       </c>
     </row>
-    <row r="291" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
         <v>1512</v>
       </c>
@@ -48526,7 +48525,7 @@
         <v>36.37122985845</v>
       </c>
     </row>
-    <row r="292" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
         <v>1518</v>
       </c>
@@ -48973,7 +48972,7 @@
         <v>36.37122985845</v>
       </c>
     </row>
-    <row r="295" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
         <v>1534</v>
       </c>
@@ -49122,7 +49121,7 @@
         <v>110.6417894474</v>
       </c>
     </row>
-    <row r="296" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
         <v>1538</v>
       </c>
@@ -49271,7 +49270,7 @@
         <v>45.023552850835998</v>
       </c>
     </row>
-    <row r="297" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
         <v>1542</v>
       </c>
@@ -49420,7 +49419,7 @@
         <v>45.023552850835998</v>
       </c>
     </row>
-    <row r="298" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
         <v>1548</v>
       </c>
@@ -49569,7 +49568,7 @@
         <v>36.37122985845</v>
       </c>
     </row>
-    <row r="299" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
         <v>1554</v>
       </c>
@@ -49718,7 +49717,7 @@
         <v>110.6417894474</v>
       </c>
     </row>
-    <row r="300" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
         <v>1558</v>
       </c>
@@ -50016,7 +50015,7 @@
         <v>110.6417894474</v>
       </c>
     </row>
-    <row r="302" spans="1:49" hidden="1" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:49" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
         <v>1568</v>
       </c>
@@ -50166,13 +50165,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AW302">
-    <filterColumn colId="20">
-      <filters>
-        <filter val="Assets/Products"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AW302"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>